<commit_message>
Added state table for line tracer manager Added new states on motor manager (fast_right, fast_left)
</commit_message>
<xml_diff>
--- a/Documents/Sumobot SRS.xlsx
+++ b/Documents/Sumobot SRS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edmar\Downloads\Code\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repository\lineTracerManager\ModSimMobot\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7452" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7452" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Revision History" sheetId="1" r:id="rId1"/>
@@ -17,11 +17,11 @@
     <sheet name="UART" sheetId="5" r:id="rId3"/>
     <sheet name="Input" sheetId="6" r:id="rId4"/>
     <sheet name="Motor" sheetId="9" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="10" r:id="rId6"/>
+    <sheet name="Line Tracer" sheetId="10" r:id="rId6"/>
     <sheet name="Schedule" sheetId="7" r:id="rId7"/>
     <sheet name="Others" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="261">
   <si>
     <r>
       <t>Software Requirement</t>
@@ -692,9 +692,6 @@
     <t>SLOW_RIGHT</t>
   </si>
   <si>
-    <t>SLOW_FORWARD</t>
-  </si>
-  <si>
     <t>FAST_FORWARD</t>
   </si>
   <si>
@@ -765,6 +762,78 @@
   </si>
   <si>
     <t>sensor_2</t>
+  </si>
+  <si>
+    <t>PARTIAL_LEFT</t>
+  </si>
+  <si>
+    <t>PARTIAL_RIGHT</t>
+  </si>
+  <si>
+    <t>HALF_LEFT</t>
+  </si>
+  <si>
+    <t>HALF_RIGHT</t>
+  </si>
+  <si>
+    <t>FULL</t>
+  </si>
+  <si>
+    <t>NO_LINE</t>
+  </si>
+  <si>
+    <t>LEGEND</t>
+  </si>
+  <si>
+    <t>RD6</t>
+  </si>
+  <si>
+    <t>sensor1</t>
+  </si>
+  <si>
+    <t>RD7</t>
+  </si>
+  <si>
+    <t>sensor2</t>
+  </si>
+  <si>
+    <t>sensor3</t>
+  </si>
+  <si>
+    <t>sensor1 and !sensor2 and !sensor3</t>
+  </si>
+  <si>
+    <t>RD5</t>
+  </si>
+  <si>
+    <t>!sensor1 and !sensor2 and sensor3</t>
+  </si>
+  <si>
+    <t>sensor1 and sensor2 and !sensor3</t>
+  </si>
+  <si>
+    <t>!sensor1 and sensor2 and sensor3</t>
+  </si>
+  <si>
+    <t>sesnsor1 and sensor2 and sensor3</t>
+  </si>
+  <si>
+    <t>[input]state = RIGHT_SIGHT or [line]state = PARTIAL_LEFT</t>
+  </si>
+  <si>
+    <t>FAST_RIGHT</t>
+  </si>
+  <si>
+    <t>FAST_LEFT</t>
+  </si>
+  <si>
+    <t>[line]state = HALF_LEFT or [line]state = FULL</t>
+  </si>
+  <si>
+    <t>[line]state = HALF_RIGHT or [line]state = FULL</t>
+  </si>
+  <si>
+    <t>[input]state = RIGHT_SIGHT or [line]state = PARTIAL_RIGHT</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1214,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1266,6 +1335,9 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1312,6 +1384,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1623,12 +1701,12 @@
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
     </row>
     <row r="7" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -1736,10 +1814,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="64"/>
+      <c r="B1" s="65"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -1748,11 +1826,11 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -2407,7 +2485,7 @@
         <v>89</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>113</v>
@@ -2422,7 +2500,7 @@
         <v>115</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2433,7 +2511,7 @@
         <v>90</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>113</v>
@@ -2448,7 +2526,7 @@
         <v>115</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2459,7 +2537,7 @@
         <v>91</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>101</v>
@@ -2474,7 +2552,7 @@
         <v>115</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2485,7 +2563,7 @@
         <v>92</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>101</v>
@@ -2500,7 +2578,7 @@
         <v>115</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2688,22 +2766,22 @@
       <c r="H7" s="14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="68"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="69"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="68"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="69"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
@@ -2740,17 +2818,17 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="77" t="s">
         <v>141</v>
       </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="77"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="77"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="78"/>
     </row>
     <row r="23" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="s">
@@ -2840,17 +2918,17 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="B27" s="77"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="78"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36" t="s">
@@ -2940,11 +3018,11 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="70"/>
-      <c r="C33" s="71"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="72"/>
     </row>
     <row r="34" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
@@ -3026,18 +3104,18 @@
       <c r="B48" s="24"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="72" t="s">
+      <c r="A49" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="72"/>
-      <c r="C49" s="72"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="73" t="s">
+      <c r="A50" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="B50" s="74"/>
-      <c r="C50" s="75"/>
+      <c r="B50" s="75"/>
+      <c r="C50" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3059,7 +3137,7 @@
   <dimension ref="C5:K15"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3211,7 +3289,7 @@
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3223,10 +3301,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="C5:L14"/>
+  <dimension ref="C5:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3235,14 +3313,14 @@
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.109375" customWidth="1"/>
-    <col min="8" max="8" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.5546875" customWidth="1"/>
-    <col min="11" max="11" width="25" customWidth="1"/>
+    <col min="11" max="13" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C5" s="16" t="s">
         <v>133</v>
       </c>
@@ -3253,7 +3331,7 @@
         <v>134</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>211</v>
@@ -3262,19 +3340,22 @@
         <v>212</v>
       </c>
       <c r="I5" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="J5" s="16" t="s">
-        <v>215</v>
-      </c>
       <c r="K5" s="39" t="s">
-        <v>223</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+      <c r="L5" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="M5" s="39" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C6" s="16" t="s">
         <v>134</v>
       </c>
@@ -3289,74 +3370,86 @@
       <c r="J6" s="35"/>
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
-    </row>
-    <row r="7" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="M6" s="35"/>
+    </row>
+    <row r="7" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C7" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H7" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="J7" s="35" t="s">
         <v>220</v>
-      </c>
-      <c r="J7" s="35" t="s">
-        <v>221</v>
       </c>
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
-    </row>
-    <row r="8" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="M7" s="35"/>
+    </row>
+    <row r="8" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C8" s="16" t="s">
         <v>211</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K8" s="35"/>
-      <c r="L8" s="14"/>
-    </row>
-    <row r="9" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L8" s="35" t="s">
+        <v>258</v>
+      </c>
+      <c r="M8" s="35" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C9" s="16" t="s">
         <v>212</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14" t="s">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K9" s="35"/>
-      <c r="L9" s="14"/>
-    </row>
-    <row r="10" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L9" s="35" t="s">
+        <v>258</v>
+      </c>
+      <c r="M9" s="35" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C10" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -3367,69 +3460,88 @@
       <c r="K10" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="L10" s="14"/>
-    </row>
-    <row r="11" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L10" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="M10" s="35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C11" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="35"/>
-      <c r="L11" s="14"/>
-    </row>
-    <row r="12" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+    </row>
+    <row r="12" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C12" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="35"/>
-      <c r="L12" s="14"/>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C13" s="16" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="G13" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>219</v>
+      </c>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
       <c r="K13" s="35"/>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C14" s="16"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="62" t="s">
+        <v>257</v>
+      </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="40"/>
+      <c r="G14" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>219</v>
+      </c>
       <c r="I14" s="40"/>
       <c r="J14" s="40"/>
       <c r="K14" s="35"/>
-      <c r="L14" s="40"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3439,13 +3551,237 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1"/>
+  <dimension ref="A5:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>252</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="I7" s="40" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>252</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="40" t="s">
+        <v>252</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="I9" s="40" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="B10" s="35"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" s="35"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>252</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="40" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="B12" s="35"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>252</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="80" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="B16" s="79" t="s">
+        <v>245</v>
+      </c>
+      <c r="C16" s="79"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>247</v>
+      </c>
+      <c r="C17" s="79"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" s="79" t="s">
+        <v>248</v>
+      </c>
+      <c r="C18" s="79"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A15:C15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3454,7 +3790,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
@@ -4062,10 +4398,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="67"/>
+      <c r="B1" s="68"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">

</xml_diff>

<commit_message>
Update on excel file (SRS)
</commit_message>
<xml_diff>
--- a/Documents/Sumobot SRS.xlsx
+++ b/Documents/Sumobot SRS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7452" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7452" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Revision History" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="262">
   <si>
     <r>
       <t>Software Requirement</t>
@@ -833,10 +833,10 @@
     <t>[line]state = HALF_RIGHT or [line]state = FULL</t>
   </si>
   <si>
-    <t>[input]state = RIGHT_SIGHT or [line]state = PARTIAL_RIGHT</t>
-  </si>
-  <si>
     <t>!sensor1 and !sensor2 and !sensor3</t>
+  </si>
+  <si>
+    <t>[input]state = LEFT_SIGHT or [line]state = PARTIAL_RIGHT</t>
   </si>
 </sst>
 </file>
@@ -3306,8 +3306,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="C5:M14"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3432,7 +3432,7 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -3508,7 +3508,7 @@
       <c r="L12" s="35"/>
       <c r="M12" s="35"/>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C13" s="16" t="s">
         <v>256</v>
       </c>
@@ -3522,12 +3522,14 @@
         <v>219</v>
       </c>
       <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
+      <c r="J13" s="35" t="s">
+        <v>220</v>
+      </c>
       <c r="K13" s="35"/>
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C14" s="62" t="s">
         <v>257</v>
       </c>
@@ -3541,7 +3543,9 @@
         <v>219</v>
       </c>
       <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
+      <c r="J14" s="35" t="s">
+        <v>220</v>
+      </c>
       <c r="K14" s="35"/>
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
@@ -3556,7 +3560,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A5:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -3644,7 +3648,7 @@
       <c r="B8" s="35"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14" t="s">
@@ -3667,7 +3671,7 @@
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>249</v>
@@ -3690,7 +3694,7 @@
       <c r="B10" s="35"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>249</v>
@@ -3712,7 +3716,7 @@
       <c r="B11" s="35"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>249</v>
@@ -3735,7 +3739,7 @@
       <c r="B12" s="35"/>
       <c r="C12" s="40"/>
       <c r="D12" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>249</v>

</xml_diff>

<commit_message>
Modify the code base on the integration testing on the hardward and line sensor
</commit_message>
<xml_diff>
--- a/Documents/Sumobot SRS.xlsx
+++ b/Documents/Sumobot SRS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repository\lineTracerManager\ModSimMobot\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repository\ModSimMobot\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="265">
   <si>
     <r>
       <t>Software Requirement</t>
@@ -698,9 +698,6 @@
     <t>BACKWARD</t>
   </si>
   <si>
-    <t>OFF</t>
-  </si>
-  <si>
     <t>[input]state = LEFT_SIGHT</t>
   </si>
   <si>
@@ -713,18 +710,12 @@
     <t>[input]state = RIGHT_SIGHT</t>
   </si>
   <si>
-    <t xml:space="preserve">[input]state = RIGHT_SIGHT and [input]state = LEFT_SIGHT  </t>
-  </si>
-  <si>
     <t>DELAY</t>
   </si>
   <si>
     <t>Delay</t>
   </si>
   <si>
-    <t>delay</t>
-  </si>
-  <si>
     <t>direction_a = A_CW , direction_b = B_CCW, pwm_a =100, pwm_b =100</t>
   </si>
   <si>
@@ -737,9 +728,6 @@
     <t>end</t>
   </si>
   <si>
-    <t>[input]state = NO_SIGHT</t>
-  </si>
-  <si>
     <t>DIR_A</t>
   </si>
   <si>
@@ -818,25 +806,46 @@
     <t>sesnsor1 and sensor2 and sensor3</t>
   </si>
   <si>
-    <t>[input]state = RIGHT_SIGHT or [line]state = PARTIAL_LEFT</t>
-  </si>
-  <si>
-    <t>FAST_RIGHT</t>
-  </si>
-  <si>
-    <t>FAST_LEFT</t>
-  </si>
-  <si>
-    <t>[line]state = HALF_LEFT or [line]state = FULL</t>
-  </si>
-  <si>
-    <t>[line]state = HALF_RIGHT or [line]state = FULL</t>
-  </si>
-  <si>
     <t>!sensor1 and !sensor2 and !sensor3</t>
   </si>
   <si>
-    <t>[input]state = LEFT_SIGHT or [line]state = PARTIAL_RIGHT</t>
+    <t>STANDBY</t>
+  </si>
+  <si>
+    <t>LINE_LEFT</t>
+  </si>
+  <si>
+    <t>LINE_RIGHT</t>
+  </si>
+  <si>
+    <t>LINE_FORWARD</t>
+  </si>
+  <si>
+    <t>LINE_BACKWARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [input]state = NO_SIGHT and ([line]state = FULL or [line]state = PARTIAL_LEFT or [line]state = PARTIAL_RIGHT or [line]state = HALF_RIGHT or [line]HALF_LEFT)</t>
+  </si>
+  <si>
+    <t>[input]state = LEFT_SIGHT or [line]state = PARTIAL_RIGHT or [line]state = HALF_RIGHT</t>
+  </si>
+  <si>
+    <t>[input]state = BOTH_SIGHT</t>
+  </si>
+  <si>
+    <t>[line]state = PARTIAL_LEFT or [line]state = HALF_LEFT or [line]state = FULL</t>
+  </si>
+  <si>
+    <t>[line]state = PARTIAL_RIGHT or [line]state = HALF_RIGHT or [line]state = FULL</t>
+  </si>
+  <si>
+    <t>[input]state = NO_SIGHT and [line]state = NO_LINE</t>
+  </si>
+  <si>
+    <t>direction_a = A_CCW , direction_b = B_CCW, pwm_a =20, pwm_b =20, delay =1 sec</t>
+  </si>
+  <si>
+    <t>direction_a = A_CCW , direction_b = B_CW, pwm_a =0, pwm_b =0, delay = 1sec, pwm_a=80, pwm_b=80, delay=3sec then change state to OFF</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1226,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1394,6 +1403,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2488,7 +2500,7 @@
         <v>89</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>113</v>
@@ -2503,7 +2515,7 @@
         <v>115</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2514,7 +2526,7 @@
         <v>90</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>113</v>
@@ -2529,7 +2541,7 @@
         <v>115</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2540,7 +2552,7 @@
         <v>91</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>101</v>
@@ -2555,7 +2567,7 @@
         <v>115</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2566,7 +2578,7 @@
         <v>92</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>101</v>
@@ -2581,7 +2593,7 @@
         <v>115</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -3292,7 +3304,7 @@
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -3304,10 +3316,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="C5:M14"/>
+  <dimension ref="C5:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3321,45 +3333,53 @@
     <col min="9" max="9" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.5546875" customWidth="1"/>
     <col min="11" max="13" width="25" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" customWidth="1"/>
+    <col min="15" max="15" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C5" s="16" t="s">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C5" s="62" t="s">
         <v>133</v>
       </c>
       <c r="D5" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="62" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="62" t="s">
         <v>212</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="62" t="s">
         <v>214</v>
       </c>
       <c r="K5" s="39" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L5" s="39" t="s">
+        <v>253</v>
+      </c>
+      <c r="M5" s="39" t="s">
+        <v>254</v>
+      </c>
+      <c r="N5" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="O5" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="M5" s="39" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C6" s="16" t="s">
+    </row>
+    <row r="6" spans="3:15" s="81" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C6" s="17" t="s">
         <v>134</v>
       </c>
       <c r="D6" s="35"/>
@@ -3374,85 +3394,90 @@
       <c r="K6" s="35"/>
       <c r="L6" s="35"/>
       <c r="M6" s="35"/>
-    </row>
-    <row r="7" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C7" s="16" t="s">
-        <v>215</v>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C7" s="62" t="s">
+        <v>252</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35" t="s">
-        <v>216</v>
+        <v>258</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J7" s="35" t="s">
-        <v>220</v>
+        <v>259</v>
       </c>
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
       <c r="M7" s="35"/>
-    </row>
-    <row r="8" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C8" s="16" t="s">
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+    </row>
+    <row r="8" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C8" s="62" t="s">
         <v>211</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="14" t="s">
-        <v>255</v>
+      <c r="H8" s="35" t="s">
+        <v>218</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="35" t="s">
-        <v>220</v>
+        <v>259</v>
       </c>
       <c r="K8" s="35"/>
-      <c r="L8" s="35" t="s">
-        <v>258</v>
-      </c>
       <c r="M8" s="35" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="9" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C9" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+    </row>
+    <row r="9" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C9" s="62" t="s">
         <v>212</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14" t="s">
-        <v>261</v>
+        <v>215</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="35" t="s">
-        <v>220</v>
+        <v>259</v>
       </c>
       <c r="K9" s="35"/>
       <c r="L9" s="35" t="s">
-        <v>258</v>
-      </c>
-      <c r="M9" s="35" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="10" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C10" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+    </row>
+    <row r="10" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C10" s="62" t="s">
         <v>214</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -3463,92 +3488,143 @@
       <c r="K10" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="L10" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="M10" s="35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C11" s="16" t="s">
-        <v>221</v>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+    </row>
+    <row r="11" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C11" s="62" t="s">
+        <v>219</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="35"/>
       <c r="L11" s="35"/>
       <c r="M11" s="35"/>
-    </row>
-    <row r="12" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C12" s="16" t="s">
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+    </row>
+    <row r="12" spans="3:15" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C12" s="62" t="s">
         <v>213</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E12" s="14"/>
-      <c r="F12" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="F12" s="35" t="s">
+        <v>262</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>218</v>
+      </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="35"/>
       <c r="L12" s="35"/>
       <c r="M12" s="35"/>
-    </row>
-    <row r="13" spans="3:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C13" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="D13" s="14"/>
+      <c r="O12" s="35" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C13" s="62" t="s">
+        <v>253</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>263</v>
+      </c>
       <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>219</v>
-      </c>
+      <c r="F13" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="40"/>
       <c r="I13" s="40"/>
-      <c r="J13" s="35" t="s">
-        <v>220</v>
-      </c>
+      <c r="J13" s="35"/>
       <c r="K13" s="35"/>
       <c r="L13" s="35"/>
       <c r="M13" s="35"/>
-    </row>
-    <row r="14" spans="3:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N13" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="O13" s="35"/>
+    </row>
+    <row r="14" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C14" s="62" t="s">
-        <v>257</v>
-      </c>
-      <c r="D14" s="14"/>
+        <v>254</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>263</v>
+      </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="H14" s="40" t="s">
-        <v>219</v>
-      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="40"/>
-      <c r="J14" s="35" t="s">
-        <v>220</v>
-      </c>
+      <c r="J14" s="35"/>
       <c r="K14" s="35"/>
       <c r="L14" s="35"/>
       <c r="M14" s="35"/>
+      <c r="N14" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="O14" s="35"/>
+    </row>
+    <row r="15" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C15" s="62" t="s">
+        <v>255</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+    </row>
+    <row r="16" spans="3:15" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C16" s="62" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3585,22 +3661,22 @@
         <v>134</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E5" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>237</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3620,172 +3696,172 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>247</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="H7" s="40" t="s">
         <v>249</v>
       </c>
-      <c r="F7" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="G7" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="H7" s="40" t="s">
-        <v>253</v>
-      </c>
       <c r="I7" s="40" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B8" s="35"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="H8" s="40" t="s">
         <v>249</v>
       </c>
-      <c r="G8" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="H8" s="40" t="s">
-        <v>253</v>
-      </c>
       <c r="I8" s="40" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="40" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I9" s="40" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B10" s="35"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E10" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="H10" s="40" t="s">
         <v>249</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="H10" s="40" t="s">
-        <v>253</v>
-      </c>
       <c r="I10" s="40" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B11" s="35"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="40" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="40"/>
       <c r="D12" s="14" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E12" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="H12" s="40" t="s">
         <v>249</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="G12" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="H12" s="40" t="s">
-        <v>253</v>
       </c>
       <c r="I12" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="80" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B15" s="80"/>
       <c r="C15" s="80"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B16" s="79" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C16" s="79"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B17" s="79" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C17" s="79"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B18" s="79" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C18" s="79"/>
     </row>

</xml_diff>

<commit_message>
updated code, added new states on motor manager to handle line tracer manager
</commit_message>
<xml_diff>
--- a/Documents/Sumobot SRS.xlsx
+++ b/Documents/Sumobot SRS.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="268">
   <si>
     <r>
       <t>Software Requirement</t>
@@ -827,9 +827,6 @@
     <t xml:space="preserve"> [input]state = NO_SIGHT and ([line]state = FULL or [line]state = PARTIAL_LEFT or [line]state = PARTIAL_RIGHT or [line]state = HALF_RIGHT or [line]HALF_LEFT)</t>
   </si>
   <si>
-    <t>[input]state = LEFT_SIGHT or [line]state = PARTIAL_RIGHT or [line]state = HALF_RIGHT</t>
-  </si>
-  <si>
     <t>[input]state = BOTH_SIGHT</t>
   </si>
   <si>
@@ -845,7 +842,19 @@
     <t>direction_a = A_CCW , direction_b = B_CCW, pwm_a =20, pwm_b =20, delay =1 sec</t>
   </si>
   <si>
-    <t>direction_a = A_CCW , direction_b = B_CW, pwm_a =0, pwm_b =0, delay = 1sec, pwm_a=80, pwm_b=80, delay=3sec then change state to OFF</t>
+    <t>direction_a = A_CCW , direction_b = B_CW, pwm_a =0, pwm_b =0, delay = 1sec, pwm_a=80, pwm_b=80, delay=3sec then change state to Standby</t>
+  </si>
+  <si>
+    <t>[input]state = LEFT_SIGHT or [line]state = PARTIAL_RIGHT or [line]state = HALF_RIGHT or [input]state = NO_SIGHT</t>
+  </si>
+  <si>
+    <t>added condiion [input]state = NO_SIGHT when on STANDBY then go to SLOW_LEFT</t>
+  </si>
+  <si>
+    <t>removed standby state on line left on code</t>
+  </si>
+  <si>
+    <t>di ko pa nalalagay tong action na to on code</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1235,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1406,6 +1415,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3316,10 +3328,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="C5:O16"/>
+  <dimension ref="C4:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3337,6 +3349,17 @@
     <col min="15" max="15" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="3:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F4" s="81" t="s">
+        <v>266</v>
+      </c>
+      <c r="G4" s="82" t="s">
+        <v>265</v>
+      </c>
+      <c r="O4" s="82" t="s">
+        <v>267</v>
+      </c>
+    </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C5" s="62" t="s">
         <v>133</v>
@@ -3409,13 +3432,13 @@
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>218</v>
       </c>
       <c r="J7" s="35" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
@@ -3438,11 +3461,11 @@
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="35" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K8" s="35"/>
       <c r="M8" s="35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N8" s="35"/>
       <c r="O8" s="35"/>
@@ -3462,11 +3485,11 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="35" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K9" s="35"/>
       <c r="L9" s="35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M9" s="35"/>
       <c r="N9" s="35"/>
@@ -3505,7 +3528,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14" t="s">
-        <v>219</v>
+        <v>160</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="35"/>
@@ -3523,7 +3546,7 @@
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="35" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G12" s="35" t="s">
         <v>215</v>
@@ -3545,7 +3568,7 @@
         <v>253</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="14" t="s">
@@ -3568,7 +3591,7 @@
         <v>254</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -3589,7 +3612,7 @@
         <v>255</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14" t="s">
@@ -3610,7 +3633,7 @@
         <v>256</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14" t="s">

</xml_diff>

<commit_message>
Last update for v0.4. Update code, working line tracer manager
</commit_message>
<xml_diff>
--- a/Documents/Sumobot SRS.xlsx
+++ b/Documents/Sumobot SRS.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="267">
   <si>
     <r>
       <t>Software Requirement</t>
@@ -701,12 +701,6 @@
     <t>[input]state = LEFT_SIGHT</t>
   </si>
   <si>
-    <t>direction_a=A_CW , direction b = B_CCW, pwm_a =0, pwm_b =0</t>
-  </si>
-  <si>
-    <t>direction_a = A_CCW , direction_b = B_CCW, pwm_a =20, pwm_b =20</t>
-  </si>
-  <si>
     <t>[input]state = RIGHT_SIGHT</t>
   </si>
   <si>
@@ -716,15 +710,6 @@
     <t>Delay</t>
   </si>
   <si>
-    <t>direction_a = A_CW , direction_b = B_CCW, pwm_a =100, pwm_b =100</t>
-  </si>
-  <si>
-    <t>direction_a = A_CCW , direction_b = B_CW, pwm_a =50, pwm_b =50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">direction_a=A_CW , direction b = B_CCW, pwm_a =0, pwm_b =0, delay = 1sec , </t>
-  </si>
-  <si>
     <t>end</t>
   </si>
   <si>
@@ -839,22 +824,34 @@
     <t>[input]state = NO_SIGHT and [line]state = NO_LINE</t>
   </si>
   <si>
-    <t>direction_a = A_CCW , direction_b = B_CCW, pwm_a =20, pwm_b =20, delay =1 sec</t>
-  </si>
-  <si>
-    <t>direction_a = A_CCW , direction_b = B_CW, pwm_a =0, pwm_b =0, delay = 1sec, pwm_a=80, pwm_b=80, delay=3sec then change state to Standby</t>
-  </si>
-  <si>
     <t>[input]state = LEFT_SIGHT or [line]state = PARTIAL_RIGHT or [line]state = HALF_RIGHT or [input]state = NO_SIGHT</t>
   </si>
   <si>
-    <t>added condiion [input]state = NO_SIGHT when on STANDBY then go to SLOW_LEFT</t>
-  </si>
-  <si>
-    <t>removed standby state on line left on code</t>
-  </si>
-  <si>
-    <t>di ko pa nalalagay tong action na to on code</t>
+    <t>direction_a = Move_Forward , direction_b = Move_Backward, pwm_a =80, pwm_b =80</t>
+  </si>
+  <si>
+    <t>direction_a = Move_Backward , direction_b = Move_Forward, pwm_a =80, pwm_b =80</t>
+  </si>
+  <si>
+    <t>direction_a = Move_Backward , direction_b = Move_Backward, pwm_a =80, pwm_b =80</t>
+  </si>
+  <si>
+    <t>Motor_Off(), pwm_a =0, pwm_b =0, delay = 0.5sec</t>
+  </si>
+  <si>
+    <t>direction_a = Move_Forward , direction_b = Move-Forward, pwm_a =100, pwm_b =100</t>
+  </si>
+  <si>
+    <t>direction_a = Move_Forward , direction_b = Move_Backward, pwm_a =80, pwm_b =80, delay = 1sec</t>
+  </si>
+  <si>
+    <t>direction_a = Move_Backward , direction_b = Move_Forward, pwm_a =80, pwm_b =80, delay = 1sec</t>
+  </si>
+  <si>
+    <t>direction_a = Move_Forward , direction_b = Move-Forward, pwm_a =80, pwm_b =80, delay = 2sec</t>
+  </si>
+  <si>
+    <t>direction_a = Move_Backward , direction_b = Move_Backward, pwm_a =80, pwm_b =80, delay = 2sec</t>
   </si>
 </sst>
 </file>
@@ -1359,6 +1356,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1412,12 +1415,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1728,12 +1725,12 @@
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
     </row>
     <row r="7" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -1841,10 +1838,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="65"/>
+      <c r="B1" s="67"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -1853,11 +1850,11 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -2512,7 +2509,7 @@
         <v>89</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>113</v>
@@ -2527,7 +2524,7 @@
         <v>115</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2538,7 +2535,7 @@
         <v>90</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>113</v>
@@ -2553,7 +2550,7 @@
         <v>115</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2564,7 +2561,7 @@
         <v>91</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>101</v>
@@ -2579,7 +2576,7 @@
         <v>115</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2590,7 +2587,7 @@
         <v>92</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>101</v>
@@ -2605,7 +2602,7 @@
         <v>115</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2793,22 +2790,22 @@
       <c r="H7" s="14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="71"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="69"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="71"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
@@ -2845,17 +2842,17 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="79" t="s">
         <v>141</v>
       </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
     </row>
     <row r="23" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="s">
@@ -2945,17 +2942,17 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="79" t="s">
         <v>152</v>
       </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36" t="s">
@@ -3045,11 +3042,11 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="70" t="s">
+      <c r="A33" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="72"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="74"/>
     </row>
     <row r="34" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
@@ -3131,18 +3128,18 @@
       <c r="B48" s="24"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="73" t="s">
+      <c r="A49" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="73"/>
-      <c r="C49" s="73"/>
+      <c r="B49" s="75"/>
+      <c r="C49" s="75"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="74" t="s">
+      <c r="A50" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="B50" s="75"/>
-      <c r="C50" s="76"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3316,7 +3313,7 @@
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3349,16 +3346,10 @@
     <col min="15" max="15" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F4" s="81" t="s">
-        <v>266</v>
-      </c>
-      <c r="G4" s="82" t="s">
-        <v>265</v>
-      </c>
-      <c r="O4" s="82" t="s">
-        <v>267</v>
-      </c>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="F4" s="63"/>
+      <c r="G4" s="64"/>
+      <c r="O4" s="64"/>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C5" s="62" t="s">
@@ -3371,7 +3362,7 @@
         <v>134</v>
       </c>
       <c r="F5" s="62" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G5" s="62" t="s">
         <v>211</v>
@@ -3386,22 +3377,22 @@
         <v>214</v>
       </c>
       <c r="K5" s="39" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L5" s="39" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="M5" s="39" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="N5" s="39" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="O5" s="39" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="3:15" s="81" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" s="63" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C6" s="17" t="s">
         <v>134</v>
       </c>
@@ -3419,26 +3410,24 @@
       <c r="M6" s="35"/>
       <c r="N6" s="35"/>
       <c r="O6" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="7" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C7" s="62" t="s">
-        <v>252</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>216</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="D7" s="35"/>
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J7" s="35" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
@@ -3451,21 +3440,21 @@
         <v>211</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>217</v>
+        <v>258</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="35" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="35" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="K8" s="35"/>
       <c r="M8" s="35" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="N8" s="35"/>
       <c r="O8" s="35"/>
@@ -3475,7 +3464,7 @@
         <v>212</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -3485,11 +3474,11 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="35" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="K9" s="35"/>
       <c r="L9" s="35" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="M9" s="35"/>
       <c r="N9" s="35"/>
@@ -3500,7 +3489,7 @@
         <v>214</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>222</v>
+        <v>260</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -3516,12 +3505,12 @@
       <c r="N10" s="35"/>
       <c r="O10" s="35"/>
     </row>
-    <row r="11" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C11" s="62" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>223</v>
+        <v>261</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -3542,17 +3531,17 @@
         <v>213</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>221</v>
+        <v>262</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="35" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="G12" s="35" t="s">
         <v>215</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -3560,20 +3549,18 @@
       <c r="L12" s="35"/>
       <c r="M12" s="35"/>
       <c r="O12" s="35" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="13" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C13" s="62" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E13" s="14"/>
-      <c r="F13" s="14" t="s">
-        <v>160</v>
-      </c>
+      <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="40"/>
       <c r="I13" s="40"/>
@@ -3586,12 +3573,12 @@
       </c>
       <c r="O13" s="35"/>
     </row>
-    <row r="14" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C14" s="62" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -3607,12 +3594,12 @@
       </c>
       <c r="O14" s="35"/>
     </row>
-    <row r="15" spans="3:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C15" s="62" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14" t="s">
@@ -3628,12 +3615,12 @@
       <c r="N15" s="35"/>
       <c r="O15" s="35"/>
     </row>
-    <row r="16" spans="3:15" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C16" s="62" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14" t="s">
@@ -3684,22 +3671,22 @@
         <v>134</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3719,174 +3706,174 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>242</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="I7" s="40" t="s">
         <v>245</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="G7" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="H7" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="I7" s="40" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B8" s="35"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="I8" s="40" t="s">
         <v>245</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="H8" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="I8" s="40" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="40" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="I9" s="40" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B10" s="35"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E10" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="I10" s="40" t="s">
         <v>245</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="H10" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="I10" s="40" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B11" s="35"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="40" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="40"/>
       <c r="D12" s="14" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="I12" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="80" t="s">
-        <v>239</v>
-      </c>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
+      <c r="A15" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" s="82"/>
+      <c r="C15" s="82"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="B16" s="79" t="s">
-        <v>241</v>
-      </c>
-      <c r="C16" s="79"/>
+        <v>235</v>
+      </c>
+      <c r="B16" s="81" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="81"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="B17" s="79" t="s">
-        <v>243</v>
-      </c>
-      <c r="C17" s="79"/>
+        <v>237</v>
+      </c>
+      <c r="B17" s="81" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17" s="81"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="B18" s="79" t="s">
-        <v>244</v>
-      </c>
-      <c r="C18" s="79"/>
+        <v>241</v>
+      </c>
+      <c r="B18" s="81" t="s">
+        <v>239</v>
+      </c>
+      <c r="C18" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4513,10 +4500,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="68"/>
+      <c r="B1" s="70"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">

</xml_diff>